<commit_message>
Added a message that says if the folder already exists
</commit_message>
<xml_diff>
--- a/assignments/assignment_5/group_3_ass_5_2023/ 2013_Abril.xlsx
+++ b/assignments/assignment_5/group_3_ass_5_2023/ 2013_Abril.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="199">
   <si>
     <t>Préstamos hasta 30 días</t>
   </si>
@@ -91,547 +91,526 @@
     <t>-</t>
   </si>
   <si>
+    <t>23.87</t>
+  </si>
+  <si>
+    <t>30.26</t>
+  </si>
+  <si>
+    <t>29.56</t>
+  </si>
+  <si>
+    <t>30.61</t>
+  </si>
+  <si>
+    <t>24.74</t>
+  </si>
+  <si>
+    <t>30.91</t>
+  </si>
+  <si>
+    <t>44.16</t>
+  </si>
+  <si>
+    <t>42.58</t>
+  </si>
+  <si>
+    <t>34.10</t>
+  </si>
+  <si>
+    <t>46.59</t>
+  </si>
+  <si>
+    <t>49.00</t>
+  </si>
+  <si>
+    <t>45.42</t>
+  </si>
+  <si>
+    <t>36.23</t>
+  </si>
+  <si>
+    <t>55.18</t>
+  </si>
+  <si>
+    <t>35.82</t>
+  </si>
+  <si>
+    <t>26.62</t>
+  </si>
+  <si>
+    <t>26.08</t>
+  </si>
+  <si>
+    <t>27.16</t>
+  </si>
+  <si>
+    <t>32.06</t>
+  </si>
+  <si>
+    <t>44.72</t>
+  </si>
+  <si>
+    <t>28.18</t>
+  </si>
+  <si>
+    <t>32.88</t>
+  </si>
+  <si>
+    <t>32.45</t>
+  </si>
+  <si>
+    <t>45.22</t>
+  </si>
+  <si>
+    <t>53.32</t>
+  </si>
+  <si>
+    <t>46.52</t>
+  </si>
+  <si>
+    <t>45.69</t>
+  </si>
+  <si>
+    <t>44.95</t>
+  </si>
+  <si>
+    <t>36.10</t>
+  </si>
+  <si>
+    <t>30.03</t>
+  </si>
+  <si>
+    <t>37.77</t>
+  </si>
+  <si>
+    <t>38.96</t>
+  </si>
+  <si>
+    <t>132.02</t>
+  </si>
+  <si>
+    <t>70.89</t>
+  </si>
+  <si>
+    <t>49.69</t>
+  </si>
+  <si>
+    <t>38.98</t>
+  </si>
+  <si>
+    <t>24.76</t>
+  </si>
+  <si>
+    <t>53.35</t>
+  </si>
+  <si>
+    <t>104.01</t>
+  </si>
+  <si>
+    <t>82.19</t>
+  </si>
+  <si>
+    <t>80.34</t>
+  </si>
+  <si>
+    <t>45.58</t>
+  </si>
+  <si>
+    <t>43.70</t>
+  </si>
+  <si>
+    <t>25.08</t>
+  </si>
+  <si>
+    <t>30.28</t>
+  </si>
+  <si>
+    <t>24.95</t>
+  </si>
+  <si>
+    <t>31.49</t>
+  </si>
+  <si>
+    <t>37.67</t>
+  </si>
+  <si>
+    <t>33.40</t>
+  </si>
+  <si>
+    <t>30.79</t>
+  </si>
+  <si>
+    <t>29.89</t>
+  </si>
+  <si>
+    <t>36.07</t>
+  </si>
+  <si>
+    <t>38.48</t>
+  </si>
+  <si>
+    <t>42.07</t>
+  </si>
+  <si>
+    <t>37.03</t>
+  </si>
+  <si>
+    <t>31.31</t>
+  </si>
+  <si>
+    <t>26.73</t>
+  </si>
+  <si>
+    <t>33.23</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>35.42</t>
+  </si>
+  <si>
+    <t>45.90</t>
+  </si>
+  <si>
+    <t>41.68</t>
+  </si>
+  <si>
+    <t>40.62</t>
+  </si>
+  <si>
+    <t>34.40</t>
+  </si>
+  <si>
+    <t>41.22</t>
+  </si>
+  <si>
+    <t>49.51</t>
+  </si>
+  <si>
+    <t>44.65</t>
+  </si>
+  <si>
+    <t>46.95</t>
+  </si>
+  <si>
+    <t>43.11</t>
+  </si>
+  <si>
+    <t>40.41</t>
+  </si>
+  <si>
+    <t>23.93</t>
+  </si>
+  <si>
+    <t>23.88</t>
+  </si>
+  <si>
+    <t>23.94</t>
+  </si>
+  <si>
+    <t>14.78</t>
+  </si>
+  <si>
+    <t>25.39</t>
+  </si>
+  <si>
+    <t>24.62</t>
+  </si>
+  <si>
+    <t>25.32</t>
+  </si>
+  <si>
+    <t>28.02</t>
+  </si>
+  <si>
+    <t>24.82</t>
+  </si>
+  <si>
+    <t>36.80</t>
+  </si>
+  <si>
+    <t>43.41</t>
+  </si>
+  <si>
+    <t>38.03</t>
+  </si>
+  <si>
+    <t>34.02</t>
+  </si>
+  <si>
+    <t>36.03</t>
+  </si>
+  <si>
+    <t>37.05</t>
+  </si>
+  <si>
+    <t>35.25</t>
+  </si>
+  <si>
+    <t>15.05</t>
+  </si>
+  <si>
+    <t>15.09</t>
+  </si>
+  <si>
+    <t>14.94</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>28.00</t>
+  </si>
+  <si>
     <t>28.47</t>
   </si>
   <si>
-    <t>42.58</t>
-  </si>
-  <si>
-    <t>31.55</t>
-  </si>
-  <si>
-    <t>26.82</t>
-  </si>
-  <si>
-    <t>32.54</t>
-  </si>
-  <si>
-    <t>27.95</t>
-  </si>
-  <si>
-    <t>42.70</t>
-  </si>
-  <si>
-    <t>34.17</t>
-  </si>
-  <si>
-    <t>46.50</t>
-  </si>
-  <si>
-    <t>45.67</t>
-  </si>
-  <si>
-    <t>43.56</t>
-  </si>
-  <si>
-    <t>36.64</t>
-  </si>
-  <si>
-    <t>52.32</t>
-  </si>
-  <si>
-    <t>36.20</t>
-  </si>
-  <si>
-    <t>24.30</t>
-  </si>
-  <si>
-    <t>24.00</t>
-  </si>
-  <si>
-    <t>23.96</t>
-  </si>
-  <si>
-    <t>22.40</t>
-  </si>
-  <si>
-    <t>32.03</t>
-  </si>
-  <si>
-    <t>35.25</t>
-  </si>
-  <si>
-    <t>28.56</t>
-  </si>
-  <si>
-    <t>33.63</t>
-  </si>
-  <si>
-    <t>32.23</t>
-  </si>
-  <si>
-    <t>45.58</t>
-  </si>
-  <si>
-    <t>61.96</t>
-  </si>
-  <si>
-    <t>48.04</t>
-  </si>
-  <si>
-    <t>48.47</t>
-  </si>
-  <si>
-    <t>50.56</t>
-  </si>
-  <si>
-    <t>44.20</t>
-  </si>
-  <si>
-    <t>36.30</t>
-  </si>
-  <si>
-    <t>25.82</t>
-  </si>
-  <si>
-    <t>44.58</t>
-  </si>
-  <si>
-    <t>112.33</t>
-  </si>
-  <si>
-    <t>59.27</t>
-  </si>
-  <si>
-    <t>40.05</t>
-  </si>
-  <si>
-    <t>36.60</t>
-  </si>
-  <si>
-    <t>29.98</t>
-  </si>
-  <si>
-    <t>53.93</t>
-  </si>
-  <si>
-    <t>107.48</t>
-  </si>
-  <si>
-    <t>107.80</t>
-  </si>
-  <si>
-    <t>72.13</t>
-  </si>
-  <si>
-    <t>46.60</t>
-  </si>
-  <si>
-    <t>44.63</t>
-  </si>
-  <si>
-    <t>27.81</t>
-  </si>
-  <si>
-    <t>25.10</t>
-  </si>
-  <si>
-    <t>28.09</t>
-  </si>
-  <si>
-    <t>22.80</t>
-  </si>
-  <si>
-    <t>22.56</t>
-  </si>
-  <si>
-    <t>37.67</t>
-  </si>
-  <si>
-    <t>20.98</t>
-  </si>
-  <si>
-    <t>27.89</t>
-  </si>
-  <si>
-    <t>34.49</t>
-  </si>
-  <si>
-    <t>35.13</t>
-  </si>
-  <si>
-    <t>29.39</t>
-  </si>
-  <si>
-    <t>30.77</t>
-  </si>
-  <si>
-    <t>27.18</t>
-  </si>
-  <si>
-    <t>34.37</t>
-  </si>
-  <si>
-    <t>51.11</t>
-  </si>
-  <si>
-    <t>40.67</t>
-  </si>
-  <si>
-    <t>37.73</t>
-  </si>
-  <si>
-    <t>38.74</t>
-  </si>
-  <si>
-    <t>32.97</t>
-  </si>
-  <si>
-    <t>34.22</t>
-  </si>
-  <si>
-    <t>42.11</t>
-  </si>
-  <si>
-    <t>33.42</t>
-  </si>
-  <si>
-    <t>35.76</t>
-  </si>
-  <si>
-    <t>43.62</t>
-  </si>
-  <si>
-    <t>45.78</t>
-  </si>
-  <si>
-    <t>39.97</t>
-  </si>
-  <si>
-    <t>34.80</t>
-  </si>
-  <si>
-    <t>43.20</t>
-  </si>
-  <si>
-    <t>49.51</t>
-  </si>
-  <si>
-    <t>49.27</t>
-  </si>
-  <si>
-    <t>45.49</t>
-  </si>
-  <si>
-    <t>44.40</t>
-  </si>
-  <si>
-    <t>42.68</t>
-  </si>
-  <si>
-    <t>28.32</t>
-  </si>
-  <si>
-    <t>27.48</t>
-  </si>
-  <si>
-    <t>14.79</t>
-  </si>
-  <si>
-    <t>25.31</t>
-  </si>
-  <si>
-    <t>24.64</t>
-  </si>
-  <si>
-    <t>25.33</t>
-  </si>
-  <si>
-    <t>28.04</t>
-  </si>
-  <si>
-    <t>24.83</t>
-  </si>
-  <si>
-    <t>36.96</t>
-  </si>
-  <si>
-    <t>42.59</t>
-  </si>
-  <si>
-    <t>43.43</t>
-  </si>
-  <si>
-    <t>38.05</t>
-  </si>
-  <si>
-    <t>34.05</t>
-  </si>
-  <si>
-    <t>36.19</t>
-  </si>
-  <si>
-    <t>37.07</t>
-  </si>
-  <si>
-    <t>35.29</t>
-  </si>
-  <si>
-    <t>15.06</t>
-  </si>
-  <si>
-    <t>15.15</t>
-  </si>
-  <si>
-    <t>14.95</t>
-  </si>
-  <si>
-    <t>15.99</t>
-  </si>
-  <si>
-    <t>28.23</t>
-  </si>
-  <si>
-    <t>24.68</t>
-  </si>
-  <si>
-    <t>24.53</t>
-  </si>
-  <si>
-    <t>30.49</t>
-  </si>
-  <si>
-    <t>28.69</t>
+    <t>24.39</t>
+  </si>
+  <si>
+    <t>20.51</t>
+  </si>
+  <si>
+    <t>32.83</t>
+  </si>
+  <si>
+    <t>29.41</t>
   </si>
   <si>
     <t>38.54</t>
   </si>
   <si>
-    <t>37.00</t>
-  </si>
-  <si>
-    <t>56.50</t>
-  </si>
-  <si>
-    <t>44.17</t>
-  </si>
-  <si>
-    <t>46.45</t>
-  </si>
-  <si>
-    <t>37.24</t>
-  </si>
-  <si>
-    <t>28.44</t>
-  </si>
-  <si>
-    <t>16.71</t>
-  </si>
-  <si>
-    <t>31.40</t>
-  </si>
-  <si>
-    <t>20.48</t>
-  </si>
-  <si>
-    <t>22.07</t>
-  </si>
-  <si>
-    <t>21.79</t>
-  </si>
-  <si>
-    <t>23.87</t>
-  </si>
-  <si>
-    <t>19.41</t>
-  </si>
-  <si>
-    <t>27.79</t>
-  </si>
-  <si>
-    <t>26.45</t>
-  </si>
-  <si>
-    <t>33.05</t>
-  </si>
-  <si>
-    <t>29.09</t>
-  </si>
-  <si>
-    <t>28.37</t>
-  </si>
-  <si>
-    <t>27.12</t>
+    <t>34.08</t>
+  </si>
+  <si>
+    <t>36.40</t>
+  </si>
+  <si>
+    <t>44.36</t>
+  </si>
+  <si>
+    <t>37.76</t>
+  </si>
+  <si>
+    <t>38.11</t>
+  </si>
+  <si>
+    <t>48.63</t>
+  </si>
+  <si>
+    <t>37.84</t>
+  </si>
+  <si>
+    <t>20.11</t>
+  </si>
+  <si>
+    <t>18.16</t>
+  </si>
+  <si>
+    <t>26.78</t>
+  </si>
+  <si>
+    <t>37.51</t>
+  </si>
+  <si>
+    <t>30.56</t>
+  </si>
+  <si>
+    <t>28.24</t>
+  </si>
+  <si>
+    <t>26.31</t>
+  </si>
+  <si>
+    <t>34.33</t>
+  </si>
+  <si>
+    <t>33.60</t>
+  </si>
+  <si>
+    <t>35.41</t>
+  </si>
+  <si>
+    <t>33.76</t>
   </si>
   <si>
     <t>35.31</t>
   </si>
   <si>
-    <t>42.98</t>
-  </si>
-  <si>
-    <t>38.12</t>
-  </si>
-  <si>
-    <t>36.29</t>
-  </si>
-  <si>
-    <t>37.94</t>
-  </si>
-  <si>
-    <t>34.81</t>
-  </si>
-  <si>
-    <t>34.75</t>
-  </si>
-  <si>
-    <t>33.02</t>
-  </si>
-  <si>
-    <t>34.91</t>
-  </si>
-  <si>
-    <t>10.03</t>
-  </si>
-  <si>
-    <t>21.81</t>
-  </si>
-  <si>
-    <t>20.76</t>
-  </si>
-  <si>
-    <t>18.92</t>
-  </si>
-  <si>
-    <t>77.00</t>
-  </si>
-  <si>
-    <t>19.21</t>
-  </si>
-  <si>
-    <t>28.13</t>
-  </si>
-  <si>
-    <t>28.29</t>
-  </si>
-  <si>
-    <t>30.45</t>
-  </si>
-  <si>
-    <t>32.11</t>
-  </si>
-  <si>
-    <t>25.09</t>
-  </si>
-  <si>
-    <t>40.73</t>
-  </si>
-  <si>
-    <t>45.93</t>
-  </si>
-  <si>
-    <t>41.32</t>
-  </si>
-  <si>
-    <t>41.88</t>
-  </si>
-  <si>
-    <t>43.60</t>
-  </si>
-  <si>
-    <t>34.82</t>
-  </si>
-  <si>
-    <t>36.74</t>
-  </si>
-  <si>
-    <t>39.75</t>
-  </si>
-  <si>
-    <t>35.21</t>
-  </si>
-  <si>
-    <t>27.67</t>
-  </si>
-  <si>
-    <t>32.93</t>
-  </si>
-  <si>
-    <t>27.59</t>
-  </si>
-  <si>
-    <t>35.55</t>
-  </si>
-  <si>
-    <t>45.00</t>
-  </si>
-  <si>
-    <t>36.56</t>
-  </si>
-  <si>
-    <t>40.66</t>
-  </si>
-  <si>
-    <t>35.00</t>
-  </si>
-  <si>
-    <t>24.21</t>
-  </si>
-  <si>
-    <t>21.57</t>
-  </si>
-  <si>
-    <t>24.33</t>
-  </si>
-  <si>
-    <t>21.09</t>
-  </si>
-  <si>
-    <t>18.90</t>
-  </si>
-  <si>
-    <t>20.67</t>
-  </si>
-  <si>
-    <t>51.50</t>
-  </si>
-  <si>
-    <t>19.29</t>
+    <t>34.25</t>
+  </si>
+  <si>
+    <t>31.99</t>
+  </si>
+  <si>
+    <t>27.26</t>
+  </si>
+  <si>
+    <t>32.68</t>
+  </si>
+  <si>
+    <t>9.81</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>20.74</t>
+  </si>
+  <si>
+    <t>23.97</t>
+  </si>
+  <si>
+    <t>26.02</t>
+  </si>
+  <si>
+    <t>20.14</t>
+  </si>
+  <si>
+    <t>21.08</t>
+  </si>
+  <si>
+    <t>29.07</t>
+  </si>
+  <si>
+    <t>36.16</t>
+  </si>
+  <si>
+    <t>29.85</t>
+  </si>
+  <si>
+    <t>31.65</t>
+  </si>
+  <si>
+    <t>31.20</t>
+  </si>
+  <si>
+    <t>26.41</t>
+  </si>
+  <si>
+    <t>42.17</t>
+  </si>
+  <si>
+    <t>46.21</t>
+  </si>
+  <si>
+    <t>38.92</t>
+  </si>
+  <si>
+    <t>43.94</t>
+  </si>
+  <si>
+    <t>42.05</t>
+  </si>
+  <si>
+    <t>36.54</t>
+  </si>
+  <si>
+    <t>40.59</t>
+  </si>
+  <si>
+    <t>34.07</t>
+  </si>
+  <si>
+    <t>22.30</t>
+  </si>
+  <si>
+    <t>27.69</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>37.22</t>
+  </si>
+  <si>
+    <t>27.25</t>
+  </si>
+  <si>
+    <t>34.94</t>
+  </si>
+  <si>
+    <t>37.57</t>
+  </si>
+  <si>
+    <t>36.72</t>
+  </si>
+  <si>
+    <t>34.27</t>
+  </si>
+  <si>
+    <t>25.60</t>
+  </si>
+  <si>
+    <t>28.67</t>
+  </si>
+  <si>
+    <t>25.43</t>
+  </si>
+  <si>
+    <t>19.23</t>
+  </si>
+  <si>
+    <t>15.83</t>
+  </si>
+  <si>
+    <t>24.26</t>
+  </si>
+  <si>
+    <t>19.40</t>
+  </si>
+  <si>
+    <t>23.30</t>
+  </si>
+  <si>
+    <t>27.44</t>
+  </si>
+  <si>
+    <t>50.37</t>
+  </si>
+  <si>
+    <t>27.28</t>
+  </si>
+  <si>
+    <t>27.91</t>
+  </si>
+  <si>
+    <t>29.75</t>
+  </si>
+  <si>
+    <t>26.74</t>
+  </si>
+  <si>
+    <t>38.26</t>
+  </si>
+  <si>
+    <t>43.23</t>
+  </si>
+  <si>
+    <t>42.02</t>
   </si>
   <si>
     <t>43.04</t>
   </si>
   <si>
-    <t>26.98</t>
-  </si>
-  <si>
-    <t>27.98</t>
-  </si>
-  <si>
-    <t>30.52</t>
-  </si>
-  <si>
-    <t>26.79</t>
-  </si>
-  <si>
-    <t>38.55</t>
-  </si>
-  <si>
-    <t>62.43</t>
-  </si>
-  <si>
-    <t>42.92</t>
-  </si>
-  <si>
-    <t>43.51</t>
-  </si>
-  <si>
-    <t>40.49</t>
-  </si>
-  <si>
-    <t>36.50</t>
-  </si>
-  <si>
-    <t>34.59</t>
-  </si>
-  <si>
-    <t>36.06</t>
-  </si>
-  <si>
-    <t>33.84</t>
-  </si>
-  <si>
-    <t>10.07</t>
+    <t>39.90</t>
+  </si>
+  <si>
+    <t>36.39</t>
+  </si>
+  <si>
+    <t>33.44</t>
+  </si>
+  <si>
+    <t>36.28</t>
+  </si>
+  <si>
+    <t>32.29</t>
+  </si>
+  <si>
+    <t>11.31</t>
   </si>
 </sst>
 </file>
@@ -1188,13 +1167,13 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1378,13 +1357,13 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="K11" t="s">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1430,37 +1409,37 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="K13" t="s">
         <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1547,7 +1526,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -1562,19 +1541,19 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I16" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
       <c r="J16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="K16" t="s">
         <v>24</v>
       </c>
       <c r="L16" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1591,7 +1570,7 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -1603,16 +1582,16 @@
         <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="J17" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="K17" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1629,28 +1608,28 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>138</v>
+        <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="K18" t="s">
         <v>24</v>
       </c>
       <c r="L18" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1658,37 +1637,37 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" t="s">
-        <v>120</v>
-      </c>
-      <c r="I19" t="s">
-        <v>139</v>
-      </c>
       <c r="J19" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="K19" t="s">
         <v>24</v>
       </c>
       <c r="L19" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1696,37 +1675,37 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I20" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="K20" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="L20" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1772,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -1781,7 +1760,7 @@
         <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -1793,16 +1772,16 @@
         <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J22" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="K22" t="s">
         <v>24</v>
       </c>
       <c r="L22" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1819,28 +1798,28 @@
         <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="K23" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="L23" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1857,28 +1836,28 @@
         <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I24" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="L24" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1895,28 +1874,28 @@
         <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="J25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="K25" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="L25" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1933,28 +1912,28 @@
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H26" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I26" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="K26" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="L26" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1971,28 +1950,28 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H27" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I27" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J27" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="K27" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L27" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2094,7 +2073,7 @@
         <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="I30" t="s">
         <v>24</v>
@@ -2106,7 +2085,7 @@
         <v>24</v>
       </c>
       <c r="L30" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2114,37 +2093,37 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
         <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
         <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="I31" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J31" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K31" t="s">
         <v>24</v>
       </c>
       <c r="L31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2152,37 +2131,37 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
         <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G32" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="H32" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I32" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J32" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K32" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="L32" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2190,37 +2169,37 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
         <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H33" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I33" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="J33" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K33" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L33" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2228,37 +2207,37 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
         <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G34" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H34" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I34" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J34" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="K34" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="L34" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2266,37 +2245,37 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
         <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H35" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="J35" t="s">
-        <v>171</v>
+        <v>24</v>
       </c>
       <c r="K35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="L35" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2304,37 +2283,37 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
         <v>68</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H36" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I36" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="J36" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="K36" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="L36" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2456,37 +2435,37 @@
         <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
         <v>69</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H40" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I40" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="J40" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="K40" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="L40" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2494,37 +2473,37 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
         <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="G41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H41" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I41" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="J41" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="K41" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="L41" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2585,22 +2564,22 @@
         <v>24</v>
       </c>
       <c r="G43" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H43" t="s">
         <v>24</v>
       </c>
       <c r="I43" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J43" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="K43" t="s">
         <v>24</v>
       </c>
       <c r="L43" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2623,22 +2602,22 @@
         <v>24</v>
       </c>
       <c r="G44" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H44" t="s">
         <v>24</v>
       </c>
       <c r="I44" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J44" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="K44" t="s">
         <v>24</v>
       </c>
       <c r="L44" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>